<commit_message>
chore!: new variables in input file template_transitory_input.xlsx
Introduced new variables in input file template_transitory_input.xlsx used if flag IADAPTIME is set to 1 or 2 to tune adaptive time step:
    * MLT_UPPER -> multiplier to increase the adaptive time step
    * MLT_LOWER -> multiplier to decrease the adaptive time step

BREAKING CHANGES: the added variables in input file template_transitory_input.xlsx could make it not compatible with older version of the code.

modified:   input_files/input_file_template/template_transitory_input.xlsx
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_transitory_input.xlsx
+++ b/source_code/input_files/input_file_template/template_transitory_input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniele.Placido\OneDrive - Politecnico di Torino\OPENSC2\Description_of_Components\input_file_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.placido\3D Objects\OPENSC2\source_code\input_files\input_file_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D5109E-AB63-44A1-879B-4250ECB3E8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06D1BC8-24A9-496E-895A-0E60028C8F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t>SIMULATION</t>
   </si>
@@ -129,6 +129,21 @@
   </si>
   <si>
     <t>template_environment_input.xlsx</t>
+  </si>
+  <si>
+    <t>MLT_UPPER</t>
+  </si>
+  <si>
+    <t>MLT_LOWER</t>
+  </si>
+  <si>
+    <t>float or str</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiplier used to tune (increase) the adaptive time step, used if flag IADAPTIME = 1 or IADAPTIME = 2; default to 1.2. Any positive real number or none. If none default value is used. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiplier used to tune (decrease) the adaptive time step, used if flag IADAPTIME = 1 or IADAPTIME = 2; default to 0.5. Any positive real number or none. If none default value is used. </t>
   </si>
 </sst>
 </file>
@@ -186,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -207,18 +222,22 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -557,13 +576,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -613,7 +632,7 @@
       <c r="D3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="8" t="str">
+      <c r="E3" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,A6,E6,A8,E8,[1]GRID!$A$4,[1]GRID!$E$4,"template")</f>
         <v>TEND_100_STPMIN_0.1_NELEMS_200_template</v>
       </c>
@@ -631,7 +650,7 @@
       <c r="D4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -639,16 +658,16 @@
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -665,7 +684,7 @@
       <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="2">
         <v>100</v>
       </c>
     </row>
@@ -682,7 +701,7 @@
       <c r="D7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="2">
         <v>0</v>
       </c>
     </row>
@@ -699,7 +718,7 @@
       <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="2">
         <v>0.1</v>
       </c>
     </row>
@@ -720,37 +739,65 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E12" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E13" s="2">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
docs: update doc in input file template_transitory_input.xlsx
Updated section note/comments in input file template_transitory_input.xlsx to introduce the new possible values of flag IADAPTIME and to better explain the use of some other values like STPMIN and STPMAX.

modified:   input_files/input_file_template/template_transitory_input.xlsx
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_transitory_input.xlsx
+++ b/source_code/input_files/input_file_template/template_transitory_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.placido\3D Objects\OPENSC2\source_code\input_files\input_file_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06D1BC8-24A9-496E-895A-0E60028C8F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8839D6F6-D5C9-4831-8E81-79B91603EFA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,9 +47,6 @@
     <t>s</t>
   </si>
   <si>
-    <t>![s] real(ncond) - simulation end time</t>
-  </si>
-  <si>
     <t>IADAPTIME</t>
   </si>
   <si>
@@ -101,21 +98,12 @@
     <t>file to define each conductor</t>
   </si>
   <si>
-    <t>flag for time adaptivity: 0 = no adaptivity (tstep=tstepmin); 1 = adaptivity on</t>
-  </si>
-  <si>
-    <t>minimum timestep</t>
-  </si>
-  <si>
     <t>time when the most refined time step is adopted</t>
   </si>
   <si>
     <t>time duration of the most time refined grid, starting STPMAX2 seconds before TIMEREF (era TAUDUM in origine)</t>
   </si>
   <si>
-    <t>maximum timestep</t>
-  </si>
-  <si>
     <t>STPMAX</t>
   </si>
   <si>
@@ -144,6 +132,18 @@
   </si>
   <si>
     <t xml:space="preserve">Multiplier used to tune (decrease) the adaptive time step, used if flag IADAPTIME = 1 or IADAPTIME = 2; default to 0.5. Any positive real number or none. If none default value is used. </t>
+  </si>
+  <si>
+    <t>Flag for time adaptivity: 0 = no adaptivity (tstep=tstepmin); 1 = adaptivity based on variation of the whole thermal-hydraulic solution; 2 = adaptivity based only on temperature variation of the thermal-hydraulic solution; -1 = adaptive time step from user defined input file (to be implemented); -2 = adaptive time step from user defined function.</t>
+  </si>
+  <si>
+    <t>Minimum time step for the thermal-hydraulic loop. Used if flag IADAPTIME = 0. Lower bound of the adaptive time step if IADAPTIME = 1 or IADAPTIME = 2</t>
+  </si>
+  <si>
+    <t>Maximum time step for the thermal-hydraulic loop. It is the Upper bound of the adaptive time step if IADAPTIME = 1 or IADAPTIME = 2</t>
+  </si>
+  <si>
+    <t>End time of the simulation</t>
   </si>
 </sst>
 </file>
@@ -201,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -238,6 +238,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -579,10 +583,10 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -598,25 +602,25 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -624,13 +628,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,A6,E6,A8,E8,[1]GRID!$A$4,[1]GRID!$E$4,"template")</f>
@@ -639,36 +643,36 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -679,61 +683,61 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="E6" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2" t="s">
+    <row r="7" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>21</v>
+      <c r="C7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2" t="s">
+    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>22</v>
+      <c r="C8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="E8" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="2" t="s">
+    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>25</v>
+      <c r="C9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="E9" s="2">
         <v>0.5</v>
@@ -741,44 +745,44 @@
     </row>
     <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>34</v>
+        <v>29</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E12" s="2">
         <v>100</v>
@@ -786,16 +790,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E13" s="2">
         <v>5</v>

</xml_diff>